<commit_message>
Aylık plan gözden geçirildi. Ağustos planı yapıldı @ozank, @furkankarakaya
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/IMMD Production/Gate Driver Test Planı.xlsx
+++ b/Project/3501/Furkan/IMMD Production/Gate Driver Test Planı.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27480" windowHeight="12915"/>
   </bookViews>
   <sheets>
     <sheet name="Test Planı" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="192">
   <si>
     <t>Test Edilecek Birim</t>
   </si>
@@ -593,6 +593,9 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Load altında testler</t>
   </si>
 </sst>
 </file>
@@ -729,7 +732,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -996,8 +999,8 @@
   </sheetPr>
   <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N92" sqref="N92"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1744,67 +1747,64 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C40" t="s">
         <v>50</v>
       </c>
       <c r="D40" t="s">
-        <v>61</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="F40" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C41" t="s">
         <v>50</v>
       </c>
       <c r="D41" t="s">
-        <v>66</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>64</v>
+        <v>72</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="F41" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
-        <v>41</v>
+      <c r="A42" s="4">
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="C42" t="s">
         <v>50</v>
       </c>
       <c r="D42" t="s">
-        <v>72</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F42" t="s">
-        <v>73</v>
+        <v>86</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
         <v>85</v>
@@ -1821,7 +1821,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
         <v>85</v>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
         <v>85</v>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
         <v>85</v>
@@ -1872,7 +1872,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
         <v>85</v>
@@ -1889,7 +1889,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
         <v>85</v>
@@ -1906,7 +1906,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
         <v>85</v>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
         <v>85</v>
@@ -1940,7 +1940,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
         <v>85</v>
@@ -1957,7 +1957,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
         <v>85</v>
@@ -1973,25 +1973,25 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
-        <v>52</v>
+      <c r="A53" s="5">
+        <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C53" t="s">
         <v>50</v>
       </c>
       <c r="D53" t="s">
-        <v>86</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>186</v>
+        <v>88</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
         <v>87</v>
@@ -2002,13 +2002,13 @@
       <c r="D54" t="s">
         <v>88</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E54" s="2" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
         <v>87</v>
@@ -2019,13 +2019,13 @@
       <c r="D55" t="s">
         <v>88</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E55" s="3" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B56" t="s">
         <v>87</v>
@@ -2036,13 +2036,13 @@
       <c r="D56" t="s">
         <v>88</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="2" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
         <v>87</v>
@@ -2053,13 +2053,13 @@
       <c r="D57" t="s">
         <v>88</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="E57" s="3" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
         <v>87</v>
@@ -2070,13 +2070,13 @@
       <c r="D58" t="s">
         <v>88</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E58" s="2" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B59" t="s">
         <v>87</v>
@@ -2087,13 +2087,13 @@
       <c r="D59" t="s">
         <v>88</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="E59" s="3" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B60" t="s">
         <v>87</v>
@@ -2104,13 +2104,13 @@
       <c r="D60" t="s">
         <v>88</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E60" s="2" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B61" t="s">
         <v>87</v>
@@ -2121,13 +2121,13 @@
       <c r="D61" t="s">
         <v>88</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E61" s="3" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B62" t="s">
         <v>87</v>
@@ -2138,13 +2138,13 @@
       <c r="D62" t="s">
         <v>88</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="2" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
         <v>87</v>
@@ -2155,30 +2155,30 @@
       <c r="D63" t="s">
         <v>88</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="E63" s="3" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="5">
-        <v>63</v>
+      <c r="A64" s="4">
+        <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C64" t="s">
         <v>50</v>
       </c>
       <c r="D64" t="s">
-        <v>88</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>187</v>
+        <v>90</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B65" t="s">
         <v>89</v>
@@ -2195,7 +2195,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B66" t="s">
         <v>89</v>
@@ -2212,7 +2212,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B67" t="s">
         <v>89</v>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B68" t="s">
         <v>89</v>
@@ -2246,7 +2246,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B69" t="s">
         <v>89</v>
@@ -2263,7 +2263,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B70" t="s">
         <v>89</v>
@@ -2280,7 +2280,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B71" t="s">
         <v>89</v>
@@ -2297,7 +2297,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B72" t="s">
         <v>89</v>
@@ -2314,7 +2314,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B73" t="s">
         <v>89</v>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B74" t="s">
         <v>89</v>
@@ -2347,697 +2347,700 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="4">
-        <v>74</v>
+      <c r="A75" s="5">
+        <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C75" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D75" t="s">
-        <v>90</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>188</v>
+        <v>92</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F75" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C76" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D76" t="s">
-        <v>92</v>
-      </c>
-      <c r="E76" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F76" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C77" t="s">
         <v>50</v>
       </c>
       <c r="D77" t="s">
-        <v>95</v>
-      </c>
-      <c r="E77" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>93</v>
       </c>
       <c r="F77" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C78" t="s">
         <v>50</v>
       </c>
       <c r="D78" t="s">
-        <v>98</v>
-      </c>
-      <c r="E78" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F78" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="5">
-        <v>78</v>
+      <c r="A79" s="4">
+        <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C79" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D79" t="s">
-        <v>101</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="F79" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C80" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D80" t="s">
-        <v>92</v>
-      </c>
-      <c r="E80" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E80" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F80" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C81" t="s">
         <v>50</v>
       </c>
       <c r="D81" t="s">
-        <v>109</v>
-      </c>
-      <c r="E81" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E81" s="3" t="s">
         <v>112</v>
       </c>
       <c r="F81" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C82" t="s">
         <v>50</v>
       </c>
       <c r="D82" t="s">
-        <v>110</v>
-      </c>
-      <c r="E82" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E82" s="2" t="s">
         <v>112</v>
       </c>
       <c r="F82" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="4">
-        <v>82</v>
+      <c r="A83" s="5">
+        <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C83" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D83" t="s">
-        <v>111</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="F83" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="C84" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="D84" t="s">
-        <v>104</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="F84" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C85" t="s">
         <v>115</v>
       </c>
       <c r="D85" t="s">
-        <v>114</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="F85" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="5">
-        <v>85</v>
+      <c r="A86" s="4">
+        <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C86" t="s">
-        <v>115</v>
+        <v>46</v>
       </c>
       <c r="D86" t="s">
-        <v>119</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>121</v>
+        <v>133</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="F86" t="s">
-        <v>120</v>
+        <v>48</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C87" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D87" t="s">
-        <v>133</v>
-      </c>
-      <c r="E87" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E87" s="3" t="s">
         <v>134</v>
       </c>
       <c r="F87" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C88" t="s">
         <v>50</v>
       </c>
       <c r="D88" t="s">
-        <v>135</v>
-      </c>
-      <c r="E88" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E88" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F88" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C89" t="s">
         <v>50</v>
       </c>
       <c r="D89" t="s">
-        <v>136</v>
-      </c>
-      <c r="E89" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E89" s="3" t="s">
         <v>134</v>
       </c>
       <c r="F89" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="4">
-        <v>89</v>
+      <c r="A90" s="5">
+        <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C90" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D90" t="s">
-        <v>137</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="F90" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C91" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D91" t="s">
-        <v>138</v>
-      </c>
-      <c r="E91" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E91" s="3" t="s">
         <v>139</v>
       </c>
       <c r="F91" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C92" t="s">
         <v>50</v>
       </c>
       <c r="D92" t="s">
-        <v>140</v>
-      </c>
-      <c r="E92" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E92" s="2" t="s">
         <v>139</v>
       </c>
       <c r="F92" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C93" t="s">
         <v>50</v>
       </c>
       <c r="D93" t="s">
-        <v>141</v>
-      </c>
-      <c r="E93" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E93" s="3" t="s">
         <v>139</v>
       </c>
       <c r="F93" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="5">
-        <v>93</v>
+      <c r="A94" s="4">
+        <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C94" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D94" t="s">
-        <v>142</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>139</v>
+        <v>143</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="F94" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C95" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="D95" t="s">
-        <v>143</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>174</v>
+        <v>144</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="F95" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C96" t="s">
         <v>115</v>
       </c>
       <c r="D96" t="s">
-        <v>144</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="F96" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="4">
-        <v>96</v>
+      <c r="A97" s="5">
+        <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="C97" t="s">
-        <v>115</v>
+        <v>46</v>
       </c>
       <c r="D97" t="s">
-        <v>145</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>147</v>
+        <v>159</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="F97" t="s">
-        <v>120</v>
+        <v>48</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C98" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D98" t="s">
-        <v>159</v>
-      </c>
-      <c r="E98" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E98" s="2" t="s">
         <v>160</v>
       </c>
       <c r="F98" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C99" t="s">
         <v>50</v>
       </c>
       <c r="D99" t="s">
-        <v>161</v>
-      </c>
-      <c r="E99" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E99" s="3" t="s">
         <v>160</v>
       </c>
       <c r="F99" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C100" t="s">
         <v>50</v>
       </c>
       <c r="D100" t="s">
-        <v>162</v>
-      </c>
-      <c r="E100" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E100" s="2" t="s">
         <v>160</v>
       </c>
       <c r="F100" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="5">
-        <v>100</v>
+      <c r="A101" s="4">
+        <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C101" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D101" t="s">
-        <v>163</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>160</v>
+        <v>164</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="F101" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C102" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D102" t="s">
-        <v>164</v>
-      </c>
-      <c r="E102" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E102" s="2" t="s">
         <v>165</v>
       </c>
       <c r="F102" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C103" t="s">
         <v>50</v>
       </c>
       <c r="D103" t="s">
-        <v>166</v>
-      </c>
-      <c r="E103" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E103" s="3" t="s">
         <v>165</v>
       </c>
       <c r="F103" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C104" t="s">
         <v>50</v>
       </c>
       <c r="D104" t="s">
-        <v>167</v>
-      </c>
-      <c r="E104" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E104" s="2" t="s">
         <v>165</v>
       </c>
       <c r="F104" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="4">
-        <v>104</v>
+      <c r="A105" s="5">
+        <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C105" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D105" t="s">
-        <v>168</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>165</v>
+        <v>169</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="F105" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C106" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="D106" t="s">
-        <v>169</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="F106" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B107" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C107" t="s">
         <v>115</v>
       </c>
       <c r="D107" t="s">
-        <v>170</v>
-      </c>
-      <c r="E107" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="F107" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="5">
-        <v>107</v>
+      <c r="A108" s="4">
+        <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="C108" t="s">
         <v>115</v>
       </c>
       <c r="D108" t="s">
-        <v>171</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>173</v>
+        <v>176</v>
+      </c>
+      <c r="E108" t="s">
+        <v>177</v>
       </c>
       <c r="F108" t="s">
-        <v>120</v>
+        <v>178</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C109" t="s">
         <v>115</v>
       </c>
       <c r="D109" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E109" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F109" t="s">
         <v>178</v>
@@ -3045,42 +3048,27 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B110" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C110" t="s">
         <v>115</v>
       </c>
       <c r="D110" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E110" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="F110" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="4">
-        <v>110</v>
-      </c>
       <c r="B111" t="s">
-        <v>185</v>
-      </c>
-      <c r="C111" t="s">
-        <v>115</v>
-      </c>
-      <c r="D111" t="s">
-        <v>181</v>
-      </c>
-      <c r="E111" t="s">
-        <v>182</v>
-      </c>
-      <c r="F111" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -3096,8 +3084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>